<commit_message>
Fazendo mais exercícios e teste de mesa
</commit_message>
<xml_diff>
--- a/TesteMesaListaLP1.xlsx
+++ b/TesteMesaListaLP1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fe8ec47f7158ce7/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9fe8ec47f7158ce7/Área de Trabalho/Fatec - Banco de Dados/Matérias/2° Semestre/Linguagem de Programação I/LP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="442" documentId="8_{B6B0E3D4-434E-4E67-BB42-77A7DEB1F05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{705E5417-838F-47A6-AD32-A444A735C00B}"/>
+  <xr:revisionPtr revIDLastSave="546" documentId="8_{B6B0E3D4-434E-4E67-BB42-77A7DEB1F05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B63F4CB7-1837-4964-83EB-3112D579DE53}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D78679F-ABD3-4FEF-94B9-B08EA140CA02}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2D78679F-ABD3-4FEF-94B9-B08EA140CA02}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="139">
   <si>
     <t>Passo</t>
   </si>
@@ -393,6 +393,66 @@
   </si>
   <si>
     <t>print carroNovo</t>
+  </si>
+  <si>
+    <t>Nomes</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>["Lucas"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus"]</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>encontrou</t>
+  </si>
+  <si>
+    <t>nomeBuscado</t>
+  </si>
+  <si>
+    <t>Saída</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus", "Jesus"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus", "Jesus", "Andre"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus", "Jesus", "Andre", "Paulo"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus", "Jesus", "Andre", "Paulo",  "Marcos"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus", "Jesus", "Andre", "Paulo",  "Marcos", "Pedro"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus", "Jesus", "Andre", "Paulo",  "Marcos", "Pedro", "Felipe"]</t>
+  </si>
+  <si>
+    <t>["Lucas", "João", "Mateus", "Jesus", "Andre", "Paulo",  "Marcos", "Pedro", "Felipe", "Tiago"]</t>
+  </si>
+  <si>
+    <t>"Jesus"</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>ACHEI</t>
   </si>
 </sst>
 </file>
@@ -781,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -826,15 +886,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -862,6 +913,39 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,6 +961,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4EE187D-C7C5-4FC0-BDCB-C6A719A9DC04}">
   <dimension ref="B1:R89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O41" sqref="O41"/>
+    <sheetView tabSelected="1" topLeftCell="I48" zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,10 +1277,10 @@
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="10" max="10" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="83.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -1201,21 +1289,21 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="I2" s="16" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+      <c r="I2" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="18"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
@@ -1242,7 +1330,7 @@
       <c r="K3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="16" t="s">
         <v>63</v>
       </c>
       <c r="M3" s="11" t="s">
@@ -1277,7 +1365,7 @@
       <c r="K4" s="2">
         <v>21</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="17">
         <v>0</v>
       </c>
       <c r="M4" s="2">
@@ -1312,7 +1400,7 @@
       <c r="K5" s="5">
         <v>21</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="18">
         <v>6</v>
       </c>
       <c r="M5" s="5">
@@ -1347,7 +1435,7 @@
       <c r="K6" s="5">
         <v>21</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="18">
         <v>6</v>
       </c>
       <c r="M6" s="5">
@@ -1382,7 +1470,7 @@
       <c r="K7" s="5">
         <v>21</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="18">
         <v>6</v>
       </c>
       <c r="M7" s="5">
@@ -1417,7 +1505,7 @@
       <c r="K8" s="8">
         <v>0</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="19">
         <v>0</v>
       </c>
       <c r="M8" s="8">
@@ -1460,18 +1548,18 @@
       <c r="F10" s="6">
         <v>10</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="18"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="27"/>
     </row>
     <row r="11" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
@@ -1498,16 +1586,16 @@
       <c r="K11" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="N11" s="19" t="s">
+      <c r="N11" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="O11" s="27" t="s">
+      <c r="O11" s="24" t="s">
         <v>76</v>
       </c>
       <c r="P11" s="11" t="s">
@@ -1536,34 +1624,34 @@
       <c r="F12" s="6">
         <v>0</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="20">
         <v>1</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="21">
         <v>1000</v>
       </c>
-      <c r="L12" s="25">
-        <v>0</v>
-      </c>
-      <c r="M12" s="25">
-        <v>0</v>
-      </c>
-      <c r="N12" s="24">
-        <v>0</v>
-      </c>
-      <c r="O12" s="25">
-        <v>0</v>
-      </c>
-      <c r="P12" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="24">
-        <v>0</v>
-      </c>
-      <c r="R12" s="26">
+      <c r="L12" s="22">
+        <v>0</v>
+      </c>
+      <c r="M12" s="22">
+        <v>0</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0</v>
+      </c>
+      <c r="O12" s="22">
+        <v>0</v>
+      </c>
+      <c r="P12" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>0</v>
+      </c>
+      <c r="R12" s="23">
         <v>0</v>
       </c>
     </row>
@@ -1592,16 +1680,16 @@
       <c r="K13" s="5">
         <v>1000</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="18">
         <v>1000</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="18">
         <v>0</v>
       </c>
       <c r="N13" s="5">
         <v>0</v>
       </c>
-      <c r="O13" s="21">
+      <c r="O13" s="18">
         <v>0</v>
       </c>
       <c r="P13" s="5">
@@ -1624,16 +1712,16 @@
       <c r="K14" s="5">
         <v>1000</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="18">
         <v>1000</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="18">
         <v>200</v>
       </c>
       <c r="N14" s="5">
         <v>0</v>
       </c>
-      <c r="O14" s="21">
+      <c r="O14" s="18">
         <v>0</v>
       </c>
       <c r="P14" s="5">
@@ -1647,12 +1735,12 @@
       </c>
     </row>
     <row r="15" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="15"/>
       <c r="I15" s="4">
         <v>4</v>
@@ -1663,16 +1751,16 @@
       <c r="K15" s="5">
         <v>1000</v>
       </c>
-      <c r="L15" s="21">
-        <v>0</v>
-      </c>
-      <c r="M15" s="21">
+      <c r="L15" s="18">
+        <v>0</v>
+      </c>
+      <c r="M15" s="18">
         <v>0</v>
       </c>
       <c r="N15" s="5">
         <v>0</v>
       </c>
-      <c r="O15" s="21">
+      <c r="O15" s="18">
         <v>0</v>
       </c>
       <c r="P15" s="5">
@@ -1708,16 +1796,16 @@
       <c r="K16" s="5">
         <v>0</v>
       </c>
-      <c r="L16" s="21">
-        <v>0</v>
-      </c>
-      <c r="M16" s="21">
+      <c r="L16" s="18">
+        <v>0</v>
+      </c>
+      <c r="M16" s="18">
         <v>200</v>
       </c>
       <c r="N16" s="5">
         <v>0</v>
       </c>
-      <c r="O16" s="21">
+      <c r="O16" s="18">
         <v>0</v>
       </c>
       <c r="P16" s="5">
@@ -1753,16 +1841,16 @@
       <c r="K17" s="5">
         <v>1000</v>
       </c>
-      <c r="L17" s="21">
+      <c r="L17" s="18">
         <v>800</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="18">
         <v>200</v>
       </c>
       <c r="N17" s="5">
         <v>0</v>
       </c>
-      <c r="O17" s="21">
+      <c r="O17" s="18">
         <v>0</v>
       </c>
       <c r="P17" s="5">
@@ -1798,16 +1886,16 @@
       <c r="K18" s="5">
         <v>0</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="18">
         <v>800</v>
       </c>
-      <c r="M18" s="21">
+      <c r="M18" s="18">
         <v>0</v>
       </c>
       <c r="N18" s="5">
         <v>0</v>
       </c>
-      <c r="O18" s="21">
+      <c r="O18" s="18">
         <v>0</v>
       </c>
       <c r="P18" s="5">
@@ -1843,16 +1931,16 @@
       <c r="K19" s="5">
         <v>1000</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="18">
         <v>800</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="18">
         <v>200</v>
       </c>
       <c r="N19" s="5">
         <v>100</v>
       </c>
-      <c r="O19" s="21">
+      <c r="O19" s="18">
         <v>0</v>
       </c>
       <c r="P19" s="5">
@@ -1888,16 +1976,16 @@
       <c r="K20" s="5">
         <v>1000</v>
       </c>
-      <c r="L20" s="21">
-        <v>0</v>
-      </c>
-      <c r="M20" s="21">
+      <c r="L20" s="18">
+        <v>0</v>
+      </c>
+      <c r="M20" s="18">
         <v>0</v>
       </c>
       <c r="N20" s="5">
         <v>0</v>
       </c>
-      <c r="O20" s="21">
+      <c r="O20" s="18">
         <v>0</v>
       </c>
       <c r="P20" s="5">
@@ -1933,16 +2021,16 @@
       <c r="K21" s="5">
         <v>0</v>
       </c>
-      <c r="L21" s="21">
-        <v>0</v>
-      </c>
-      <c r="M21" s="21">
+      <c r="L21" s="18">
+        <v>0</v>
+      </c>
+      <c r="M21" s="18">
         <v>200</v>
       </c>
       <c r="N21" s="5">
         <v>0</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="18">
         <v>0</v>
       </c>
       <c r="P21" s="5">
@@ -1978,16 +2066,16 @@
       <c r="K22" s="5">
         <v>0</v>
       </c>
-      <c r="L22" s="21">
-        <v>0</v>
-      </c>
-      <c r="M22" s="21">
+      <c r="L22" s="18">
+        <v>0</v>
+      </c>
+      <c r="M22" s="18">
         <v>0</v>
       </c>
       <c r="N22" s="5">
         <v>100</v>
       </c>
-      <c r="O22" s="21">
+      <c r="O22" s="18">
         <v>0</v>
       </c>
       <c r="P22" s="5">
@@ -2010,16 +2098,16 @@
       <c r="K23" s="5">
         <v>1000</v>
       </c>
-      <c r="L23" s="21">
+      <c r="L23" s="18">
         <v>700</v>
       </c>
-      <c r="M23" s="21">
+      <c r="M23" s="18">
         <v>200</v>
       </c>
       <c r="N23" s="5">
         <v>100</v>
       </c>
-      <c r="O23" s="21">
+      <c r="O23" s="18">
         <v>0</v>
       </c>
       <c r="P23" s="5">
@@ -2033,13 +2121,13 @@
       </c>
     </row>
     <row r="24" spans="2:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="27"/>
       <c r="I24" s="4">
         <v>13</v>
       </c>
@@ -2049,16 +2137,16 @@
       <c r="K24" s="5">
         <v>1000</v>
       </c>
-      <c r="L24" s="21">
+      <c r="L24" s="18">
         <v>700</v>
       </c>
-      <c r="M24" s="21">
+      <c r="M24" s="18">
         <v>200</v>
       </c>
       <c r="N24" s="5">
         <v>100</v>
       </c>
-      <c r="O24" s="21">
+      <c r="O24" s="18">
         <v>700</v>
       </c>
       <c r="P24" s="5">
@@ -2096,16 +2184,16 @@
       <c r="K25" s="5">
         <v>0</v>
       </c>
-      <c r="L25" s="21">
-        <v>0</v>
-      </c>
-      <c r="M25" s="21">
+      <c r="L25" s="18">
+        <v>0</v>
+      </c>
+      <c r="M25" s="18">
         <v>0</v>
       </c>
       <c r="N25" s="5">
         <v>0</v>
       </c>
-      <c r="O25" s="21">
+      <c r="O25" s="18">
         <v>700</v>
       </c>
       <c r="P25" s="5">
@@ -2143,16 +2231,16 @@
       <c r="K26" s="5">
         <v>1000</v>
       </c>
-      <c r="L26" s="21">
+      <c r="L26" s="18">
         <v>700</v>
       </c>
-      <c r="M26" s="21">
+      <c r="M26" s="18">
         <v>200</v>
       </c>
       <c r="N26" s="5">
         <v>100</v>
       </c>
-      <c r="O26" s="21">
+      <c r="O26" s="18">
         <v>700</v>
       </c>
       <c r="P26" s="5">
@@ -2190,16 +2278,16 @@
       <c r="K27" s="5">
         <v>1000</v>
       </c>
-      <c r="L27" s="21">
+      <c r="L27" s="18">
         <v>700</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M27" s="18">
         <v>200</v>
       </c>
       <c r="N27" s="5">
         <v>100</v>
       </c>
-      <c r="O27" s="21">
+      <c r="O27" s="18">
         <v>700</v>
       </c>
       <c r="P27" s="5">
@@ -2237,16 +2325,16 @@
       <c r="K28" s="5">
         <v>1000</v>
       </c>
-      <c r="L28" s="21">
+      <c r="L28" s="18">
         <v>700</v>
       </c>
-      <c r="M28" s="21">
+      <c r="M28" s="18">
         <v>200</v>
       </c>
       <c r="N28" s="5">
         <v>100</v>
       </c>
-      <c r="O28" s="21">
+      <c r="O28" s="18">
         <v>700</v>
       </c>
       <c r="P28" s="5">
@@ -2284,16 +2372,16 @@
       <c r="K29" s="5">
         <v>0</v>
       </c>
-      <c r="L29" s="21">
-        <v>0</v>
-      </c>
-      <c r="M29" s="21">
+      <c r="L29" s="18">
+        <v>0</v>
+      </c>
+      <c r="M29" s="18">
         <v>0</v>
       </c>
       <c r="N29" s="5">
         <v>0</v>
       </c>
-      <c r="O29" s="21">
+      <c r="O29" s="18">
         <v>0</v>
       </c>
       <c r="P29" s="5">
@@ -2331,16 +2419,16 @@
       <c r="K30" s="5">
         <v>0</v>
       </c>
-      <c r="L30" s="21">
-        <v>0</v>
-      </c>
-      <c r="M30" s="21">
+      <c r="L30" s="18">
+        <v>0</v>
+      </c>
+      <c r="M30" s="18">
         <v>0</v>
       </c>
       <c r="N30" s="5">
         <v>0</v>
       </c>
-      <c r="O30" s="21">
+      <c r="O30" s="18">
         <v>0</v>
       </c>
       <c r="P30" s="5">
@@ -2378,16 +2466,16 @@
       <c r="K31" s="5">
         <v>0</v>
       </c>
-      <c r="L31" s="21">
-        <v>0</v>
-      </c>
-      <c r="M31" s="21">
+      <c r="L31" s="18">
+        <v>0</v>
+      </c>
+      <c r="M31" s="18">
         <v>0</v>
       </c>
       <c r="N31" s="5">
         <v>0</v>
       </c>
-      <c r="O31" s="21">
+      <c r="O31" s="18">
         <v>0</v>
       </c>
       <c r="P31" s="5">
@@ -2425,16 +2513,16 @@
       <c r="K32" s="8">
         <v>0</v>
       </c>
-      <c r="L32" s="22">
-        <v>0</v>
-      </c>
-      <c r="M32" s="22">
+      <c r="L32" s="19">
+        <v>0</v>
+      </c>
+      <c r="M32" s="19">
         <v>0</v>
       </c>
       <c r="N32" s="8">
         <v>0</v>
       </c>
-      <c r="O32" s="22">
+      <c r="O32" s="19">
         <v>0</v>
       </c>
       <c r="P32" s="8">
@@ -2480,13 +2568,13 @@
       <c r="F34" s="9">
         <v>40</v>
       </c>
-      <c r="I34" s="16" t="s">
+      <c r="I34" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="18"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="27"/>
     </row>
     <row r="35" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I35" s="10" t="s">
@@ -2506,26 +2594,26 @@
       </c>
     </row>
     <row r="36" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="18"/>
-      <c r="I36" s="23">
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
+      <c r="I36" s="20">
         <v>1</v>
       </c>
-      <c r="J36" s="24" t="s">
+      <c r="J36" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="K36" s="24">
+      <c r="K36" s="21">
         <v>1000</v>
       </c>
-      <c r="L36" s="24">
-        <v>0</v>
-      </c>
-      <c r="M36" s="26">
+      <c r="L36" s="21">
+        <v>0</v>
+      </c>
+      <c r="M36" s="23">
         <v>0</v>
       </c>
     </row>
@@ -2658,14 +2746,14 @@
       <c r="F41" s="6">
         <v>10</v>
       </c>
-      <c r="I41" s="16" t="s">
+      <c r="I41" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17"/>
-      <c r="N41" s="18"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="27"/>
     </row>
     <row r="42" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="4">
@@ -2718,22 +2806,22 @@
       <c r="F43" s="6">
         <v>10</v>
       </c>
-      <c r="I43" s="23">
+      <c r="I43" s="20">
         <v>1</v>
       </c>
-      <c r="J43" s="24" t="s">
+      <c r="J43" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="K43" s="24">
+      <c r="K43" s="21">
         <v>10000</v>
       </c>
-      <c r="L43" s="24">
-        <v>0</v>
-      </c>
-      <c r="M43" s="24">
-        <v>0</v>
-      </c>
-      <c r="N43" s="26">
+      <c r="L43" s="21">
+        <v>0</v>
+      </c>
+      <c r="M43" s="21">
+        <v>0</v>
+      </c>
+      <c r="N43" s="23">
         <v>0</v>
       </c>
     </row>
@@ -2793,12 +2881,12 @@
       </c>
     </row>
     <row r="46" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="18"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
       <c r="I46" s="4">
         <v>4</v>
       </c>
@@ -2928,7 +3016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="4">
         <v>4</v>
       </c>
@@ -2942,7 +3030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="4">
         <v>5</v>
       </c>
@@ -2954,6 +3042,24 @@
       </c>
       <c r="E52" s="6">
         <v>13</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="L52" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="M52" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="N52" s="11" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
@@ -2969,6 +3075,16 @@
       <c r="E53" s="6">
         <v>0</v>
       </c>
+      <c r="I53" s="20">
+        <v>1</v>
+      </c>
+      <c r="J53" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="32"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" s="4">
@@ -2983,6 +3099,18 @@
       <c r="E54" s="6">
         <v>13</v>
       </c>
+      <c r="I54" s="4">
+        <v>2</v>
+      </c>
+      <c r="J54" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="K54" s="29">
+        <v>0</v>
+      </c>
+      <c r="L54" s="29"/>
+      <c r="M54" s="29"/>
+      <c r="N54" s="33"/>
     </row>
     <row r="55" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="7">
@@ -2997,16 +3125,53 @@
       <c r="E55" s="9">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="I55" s="4">
+        <v>3</v>
+      </c>
+      <c r="J55" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="K55" s="29">
+        <v>1</v>
+      </c>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="33"/>
+    </row>
+    <row r="56" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I56" s="4">
+        <v>4</v>
+      </c>
+      <c r="J56" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="K56" s="29">
+        <v>2</v>
+      </c>
+      <c r="L56" s="29"/>
+      <c r="M56" s="29"/>
+      <c r="N56" s="33"/>
+    </row>
     <row r="57" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="18"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="27"/>
+      <c r="I57" s="4">
+        <v>5</v>
+      </c>
+      <c r="J57" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="K57" s="29">
+        <v>3</v>
+      </c>
+      <c r="L57" s="29"/>
+      <c r="M57" s="29"/>
+      <c r="N57" s="33"/>
     </row>
     <row r="58" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
@@ -3024,6 +3189,18 @@
       <c r="F58" s="12" t="s">
         <v>19</v>
       </c>
+      <c r="I58" s="4">
+        <v>6</v>
+      </c>
+      <c r="J58" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K58" s="29">
+        <v>4</v>
+      </c>
+      <c r="L58" s="29"/>
+      <c r="M58" s="29"/>
+      <c r="N58" s="33"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
@@ -3041,6 +3218,18 @@
       <c r="F59" s="3">
         <v>0</v>
       </c>
+      <c r="I59" s="4">
+        <v>7</v>
+      </c>
+      <c r="J59" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="K59" s="29">
+        <v>5</v>
+      </c>
+      <c r="L59" s="29"/>
+      <c r="M59" s="29"/>
+      <c r="N59" s="33"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" s="4">
@@ -3058,6 +3247,18 @@
       <c r="F60" s="6">
         <v>0</v>
       </c>
+      <c r="I60" s="4">
+        <v>8</v>
+      </c>
+      <c r="J60" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="K60" s="29">
+        <v>6</v>
+      </c>
+      <c r="L60" s="29"/>
+      <c r="M60" s="29"/>
+      <c r="N60" s="33"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="4">
@@ -3075,6 +3276,18 @@
       <c r="F61" s="6">
         <v>0</v>
       </c>
+      <c r="I61" s="4">
+        <v>9</v>
+      </c>
+      <c r="J61" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="K61" s="29">
+        <v>7</v>
+      </c>
+      <c r="L61" s="29"/>
+      <c r="M61" s="29"/>
+      <c r="N61" s="33"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="4">
@@ -3092,6 +3305,18 @@
       <c r="F62" s="6">
         <v>15</v>
       </c>
+      <c r="I62" s="4">
+        <v>10</v>
+      </c>
+      <c r="J62" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="K62" s="29">
+        <v>8</v>
+      </c>
+      <c r="L62" s="29"/>
+      <c r="M62" s="29"/>
+      <c r="N62" s="33"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="4">
@@ -3109,6 +3334,18 @@
       <c r="F63" s="6">
         <v>15</v>
       </c>
+      <c r="I63" s="4">
+        <v>11</v>
+      </c>
+      <c r="J63" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="K63" s="29">
+        <v>9</v>
+      </c>
+      <c r="L63" s="29"/>
+      <c r="M63" s="29"/>
+      <c r="N63" s="33"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B64" s="4">
@@ -3126,8 +3363,18 @@
       <c r="F64" s="6">
         <v>15</v>
       </c>
-    </row>
-    <row r="65" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I64" s="4">
+        <v>12</v>
+      </c>
+      <c r="J64" s="29"/>
+      <c r="K64" s="29"/>
+      <c r="L64" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="M64" s="29"/>
+      <c r="N64" s="33"/>
+    </row>
+    <row r="65" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="7">
         <v>7</v>
       </c>
@@ -3143,18 +3390,55 @@
       <c r="F65" s="9">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="16" t="s">
+      <c r="I65" s="4">
+        <v>13</v>
+      </c>
+      <c r="J65" s="29"/>
+      <c r="K65" s="29"/>
+      <c r="L65" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="M65" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="N65" s="33"/>
+    </row>
+    <row r="66" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I66" s="4">
+        <v>14</v>
+      </c>
+      <c r="J66" s="29"/>
+      <c r="K66" s="29">
+        <v>0</v>
+      </c>
+      <c r="L66" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="M66" s="29"/>
+      <c r="N66" s="33"/>
+    </row>
+    <row r="67" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="18"/>
-    </row>
-    <row r="68" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="27"/>
+      <c r="I67" s="4">
+        <v>15</v>
+      </c>
+      <c r="J67" s="29"/>
+      <c r="K67" s="29">
+        <v>1</v>
+      </c>
+      <c r="L67" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="M67" s="29"/>
+      <c r="N67" s="33"/>
+    </row>
+    <row r="68" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="10" t="s">
         <v>0</v>
       </c>
@@ -3170,8 +3454,20 @@
       <c r="F68" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I68" s="4">
+        <v>16</v>
+      </c>
+      <c r="J68" s="29"/>
+      <c r="K68" s="29">
+        <v>2</v>
+      </c>
+      <c r="L68" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="M68" s="29"/>
+      <c r="N68" s="33"/>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>1</v>
       </c>
@@ -3187,8 +3483,20 @@
       <c r="F69" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I69" s="4">
+        <v>17</v>
+      </c>
+      <c r="J69" s="29"/>
+      <c r="K69" s="29">
+        <v>3</v>
+      </c>
+      <c r="L69" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="M69" s="29"/>
+      <c r="N69" s="33"/>
+    </row>
+    <row r="70" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
         <v>2</v>
       </c>
@@ -3204,8 +3512,18 @@
       <c r="F70" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I70" s="7">
+        <v>18</v>
+      </c>
+      <c r="J70" s="34"/>
+      <c r="K70" s="34"/>
+      <c r="L70" s="34"/>
+      <c r="M70" s="34"/>
+      <c r="N70" s="35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" s="4">
         <v>3</v>
       </c>
@@ -3221,8 +3539,14 @@
       <c r="F71" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I71" s="30"/>
+      <c r="J71" s="31"/>
+      <c r="K71" s="31"/>
+      <c r="L71" s="31"/>
+      <c r="M71" s="31"/>
+      <c r="N71" s="31"/>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" s="4">
         <v>4</v>
       </c>
@@ -3238,8 +3562,14 @@
       <c r="F72" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I72" s="30"/>
+      <c r="J72" s="31"/>
+      <c r="K72" s="31"/>
+      <c r="L72" s="31"/>
+      <c r="M72" s="31"/>
+      <c r="N72" s="31"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" s="4">
         <v>5</v>
       </c>
@@ -3255,8 +3585,14 @@
       <c r="F73" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I73" s="30"/>
+      <c r="J73" s="31"/>
+      <c r="K73" s="31"/>
+      <c r="L73" s="31"/>
+      <c r="M73" s="31"/>
+      <c r="N73" s="31"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" s="4">
         <v>6</v>
       </c>
@@ -3272,8 +3608,14 @@
       <c r="F74" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I74" s="30"/>
+      <c r="J74" s="31"/>
+      <c r="K74" s="31"/>
+      <c r="L74" s="31"/>
+      <c r="M74" s="31"/>
+      <c r="N74" s="31"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" s="4">
         <v>7</v>
       </c>
@@ -3289,8 +3631,14 @@
       <c r="F75" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I75" s="30"/>
+      <c r="J75" s="31"/>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31"/>
+      <c r="M75" s="31"/>
+      <c r="N75" s="31"/>
+    </row>
+    <row r="76" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="7">
         <v>8</v>
       </c>
@@ -3307,16 +3655,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="16" t="s">
+    <row r="77" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="E78" s="18"/>
-    </row>
-    <row r="79" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="27"/>
+    </row>
+    <row r="79" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="10" t="s">
         <v>0</v>
       </c>
@@ -3330,7 +3678,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
         <v>1</v>
       </c>
@@ -3374,13 +3722,13 @@
     </row>
     <row r="83" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="84" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="18"/>
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="27"/>
     </row>
     <row r="85" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="10" t="s">
@@ -3469,11 +3817,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="I34:M34"/>
-    <mergeCell ref="I41:N41"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="I10:R10"/>
-    <mergeCell ref="B57:F57"/>
     <mergeCell ref="B67:F67"/>
     <mergeCell ref="B78:E78"/>
     <mergeCell ref="B84:F84"/>
@@ -3482,6 +3825,11 @@
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B46:E46"/>
+    <mergeCell ref="I34:M34"/>
+    <mergeCell ref="I41:N41"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I10:R10"/>
+    <mergeCell ref="B57:F57"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>